<commit_message>
adding time tracking data
</commit_message>
<xml_diff>
--- a/Sleepdata.xlsx
+++ b/Sleepdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\songy\MyPowerBI\Data-analysis-tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8877D4-F3D5-466C-8799-16E103E87420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7418E289-45CC-4A35-A9C4-B1A7809AC983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="11295" xr2:uid="{E6631801-D2CE-415F-939D-CD0A36901A92}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="28800" windowHeight="11295" activeTab="1" xr2:uid="{E6631801-D2CE-415F-939D-CD0A36901A92}"/>
   </bookViews>
   <sheets>
     <sheet name="Sleep_data" sheetId="1" r:id="rId1"/>
+    <sheet name="Time_tracking" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Time to bed</t>
   </si>
@@ -51,6 +52,63 @@
   </si>
   <si>
     <t xml:space="preserve">Night temperature </t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Hobby</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Cooking</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Weekday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
   </si>
 </sst>
 </file>
@@ -59,13 +117,19 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="170" formatCode="[$-409]h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,12 +155,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAAD95F7-8B00-436C-A024-7B65A0A47133}">
   <dimension ref="B2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,4 +535,138 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FD8227-BBDD-4C3F-AE36-92972A11A24C}">
+  <dimension ref="A2:N8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <f ca="1">TODAY()</f>
+        <v>45327</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1.75</v>
+      </c>
+      <c r="K3" s="6">
+        <v>7</v>
+      </c>
+      <c r="L3" s="6">
+        <v>8</v>
+      </c>
+      <c r="M3" s="6">
+        <f>24-SUM(C3:L3)</f>
+        <v>1.3999999999999986</v>
+      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>